<commit_message>
updates to test schedule
</commit_message>
<xml_diff>
--- a/Test-Schedule.xlsx
+++ b/Test-Schedule.xlsx
@@ -95,7 +95,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -103,15 +103,165 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +545,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,94 +554,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="C16" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>